<commit_message>
further tweak biome bonuses
</commit_message>
<xml_diff>
--- a/Research/7-days-to-die-a20-loot.xlsx
+++ b/Research/7-days-to-die-a20-loot.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">Constant</t>
+    <t xml:space="preserve">Variables</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -55,13 +55,49 @@
     <t xml:space="preserve">Wasteland</t>
   </si>
   <si>
-    <t xml:space="preserve">Container Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Container Bonus</t>
+    <t xml:space="preserve">Added Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⬅️ max 40% // 20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⬅️ max 16.2 // 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustment</t>
   </si>
   <si>
     <t xml:space="preserve">Safes/Quest Loot provide 5% + 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eye Kandy provides 10% + 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3+5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Googles provide between 3 and 5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucky Looter adds between 5% and 25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AFTER ADJUSTMENTS: Now level 300 actually feels like an achievement! As the player grows, loot stage with smoothly grow along with him – introducing new gear and gear levels slowly over almost the entire journey! Also, exploring different biomes will have a meaningful impact and the Forest Loot will always remain low even for level 300s.</t>
   </si>
 </sst>
 </file>
@@ -231,7 +267,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,6 +288,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +304,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -284,8 +328,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -298,6 +350,10 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -464,22 +520,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>213</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>226</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>239</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>252</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>265</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,22 +622,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>310</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>323</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>336</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>349</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>362</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,22 +724,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>420</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>433</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>446</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>459</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>472</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>485</c:v>
+                  <c:v>245</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -770,22 +826,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>530</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>543</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>556</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>569</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>582</c:v>
+                  <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>595</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -793,11 +849,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="26897511"/>
-        <c:axId val="44278125"/>
+        <c:axId val="70248339"/>
+        <c:axId val="53361434"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26897511"/>
+        <c:axId val="70248339"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,7 +909,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44278125"/>
+        <c:crossAx val="53361434"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -861,7 +917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44278125"/>
+        <c:axId val="53361434"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +982,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26897511"/>
+        <c:crossAx val="70248339"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1014,7 +1070,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
@@ -1024,9 +1080,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="4.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,254 +1090,421 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="n">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
       <c r="E1" s="3" t="n">
-        <v>0.5</v>
+        <v>-0.6</v>
       </c>
       <c r="F1" s="3" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8" t="n">
         <v>20</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>200</v>
-      </c>
-      <c r="K2" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="n">
+      <c r="J3" s="13" t="n">
         <v>0</v>
       </c>
+      <c r="K3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="14" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">$J$2*(1+$A4+D$1+$J$3)+($B4+D$2+$J$4)</f>
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">$J$2*(1+$A4+E$1+$J$3)+($B4+E$2+$J$4)</f>
-        <v>310</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">$J$2*(1+$A4+F$1+$J$3)+($B4+F$2+$J$4)</f>
-        <v>420</v>
-      </c>
-      <c r="G4" s="7" t="n">
+        <v>205</v>
+      </c>
+      <c r="G4" s="8" t="n">
         <f aca="false">$J$2*(1+$A4+G$1+$J$3)+($B4+G$2+$J$4)</f>
-        <v>530</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="5" t="n">
+        <v>260</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="6" t="n">
         <v>0</v>
       </c>
+      <c r="K4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="B5" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="12" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="B5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">$J$2*(1+$A5+D$1+$J$3)+($B5+D$2+$J$4)</f>
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">$J$2*(1+$A5+E$1+$J$3)+($B5+E$2+$J$4)</f>
-        <v>323</v>
+        <v>158</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">$J$2*(1+$A5+F$1+$J$3)+($B5+F$2+$J$4)</f>
-        <v>433</v>
-      </c>
-      <c r="G5" s="7" t="n">
+        <v>213</v>
+      </c>
+      <c r="G5" s="8" t="n">
         <f aca="false">$J$2*(1+$A5+G$1+$J$3)+($B5+G$2+$J$4)</f>
-        <v>543</v>
+        <v>268</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B6" s="7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="12" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="14" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">$J$2*(1+$A6+D$1+$J$3)+($B6+D$2+$J$4)</f>
-        <v>226</v>
+        <v>111</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">$J$2*(1+$A6+E$1+$J$3)+($B6+E$2+$J$4)</f>
-        <v>336</v>
+        <v>166</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">$J$2*(1+$A6+F$1+$J$3)+($B6+F$2+$J$4)</f>
-        <v>446</v>
-      </c>
-      <c r="G6" s="7" t="n">
+        <v>221</v>
+      </c>
+      <c r="G6" s="8" t="n">
         <f aca="false">$J$2*(1+$A6+G$1+$J$3)+($B6+G$2+$J$4)</f>
-        <v>556</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="13"/>
+        <v>276</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="B7" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" s="12" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="n">
         <f aca="false">$J$2*(1+$A7+D$1+$J$3)+($B7+D$2+$J$4)</f>
-        <v>239</v>
+        <v>119</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">$J$2*(1+$A7+E$1+$J$3)+($B7+E$2+$J$4)</f>
-        <v>349</v>
+        <v>174</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">$J$2*(1+$A7+F$1+$J$3)+($B7+F$2+$J$4)</f>
-        <v>459</v>
-      </c>
-      <c r="G7" s="7" t="n">
+        <v>229</v>
+      </c>
+      <c r="G7" s="8" t="n">
         <f aca="false">$J$2*(1+$A7+G$1+$J$3)+($B7+G$2+$J$4)</f>
-        <v>569</v>
+        <v>284</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="B8" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="C8" s="12" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="14" t="n">
         <v>4</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">$J$2*(1+$A8+D$1+$J$3)+($B8+D$2+$J$4)</f>
-        <v>252</v>
+        <v>127</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">$J$2*(1+$A8+E$1+$J$3)+($B8+E$2+$J$4)</f>
-        <v>362</v>
+        <v>182</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">$J$2*(1+$A8+F$1+$J$3)+($B8+F$2+$J$4)</f>
-        <v>472</v>
-      </c>
-      <c r="G8" s="7" t="n">
+        <v>237</v>
+      </c>
+      <c r="G8" s="8" t="n">
         <f aca="false">$J$2*(1+$A8+G$1+$J$3)+($B8+G$2+$J$4)</f>
-        <v>582</v>
+        <v>292</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="C9" s="15" t="n">
+      <c r="A9" s="18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="19" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="20" t="n">
         <f aca="false">$J$2*(1+$A9+D$1+$J$3)+($B9+D$2+$J$4)</f>
-        <v>265</v>
-      </c>
-      <c r="E9" s="16" t="n">
+        <v>135</v>
+      </c>
+      <c r="E9" s="20" t="n">
         <f aca="false">$J$2*(1+$A9+E$1+$J$3)+($B9+E$2+$J$4)</f>
-        <v>375</v>
-      </c>
-      <c r="F9" s="16" t="n">
+        <v>190</v>
+      </c>
+      <c r="F9" s="20" t="n">
         <f aca="false">$J$2*(1+$A9+F$1+$J$3)+($B9+F$2+$J$4)</f>
-        <v>485</v>
-      </c>
-      <c r="G9" s="6" t="n">
+        <v>245</v>
+      </c>
+      <c r="G9" s="7" t="n">
         <f aca="false">$J$2*(1+$A9+G$1+$J$3)+($B9+G$2+$J$4)</f>
-        <v>595</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I6:J6"/>
+  <mergeCells count="10">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="J11:L30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>